<commit_message>
Prefix - Name - check unique
</commit_message>
<xml_diff>
--- a/out/10_Tags.xlsx
+++ b/out/10_Tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="321">
   <si>
     <t>Name</t>
   </si>
@@ -49,99 +49,174 @@
     <t>BelongsToUnit</t>
   </si>
   <si>
-    <t>GN-vsen_holdface_HP_open</t>
-  </si>
-  <si>
-    <t>GN-vsen_holdface_WP_close</t>
-  </si>
-  <si>
-    <t>GN-ez_holdface_HP_open</t>
-  </si>
-  <si>
-    <t>GN-ez_holdface_WP_close</t>
-  </si>
-  <si>
-    <t>GN-ez_holdface_IDLE</t>
-  </si>
-  <si>
-    <t>ST1-vsen_blockade_left_HP_down</t>
-  </si>
-  <si>
-    <t>ST1-vsen_blockade_left_WP_up</t>
-  </si>
-  <si>
-    <t>ST1-ez_blockade_left_HP_down</t>
-  </si>
-  <si>
-    <t>ST1-ez_blockade_left_WP_up</t>
-  </si>
-  <si>
-    <t>ST1-vsen_blockade_right_HP_down</t>
-  </si>
-  <si>
-    <t>ST1-vsen_blockade_right_WP_up</t>
-  </si>
-  <si>
-    <t>ST1-ez_blockade_right_HP_down</t>
-  </si>
-  <si>
-    <t>ST1-ez_blockade_right_WP_up</t>
-  </si>
-  <si>
-    <t>A-sen_scanner_left</t>
-  </si>
-  <si>
-    <t>A-sen_scanner_right</t>
-  </si>
-  <si>
-    <t>GN-sen_frame_screw_left</t>
-  </si>
-  <si>
-    <t>GN-sen_frame_screw_right</t>
-  </si>
-  <si>
-    <t>GN-sen_generator_screw</t>
-  </si>
-  <si>
-    <t>OETIKER_position_hp</t>
-  </si>
-  <si>
-    <t>OETIKER_position_2mm</t>
-  </si>
-  <si>
-    <t>OETIKER_position_4mm</t>
-  </si>
-  <si>
-    <t>OETIKER_position_tensometer</t>
-  </si>
-  <si>
-    <t>OETIKER_position_band_left_hp</t>
-  </si>
-  <si>
-    <t>OETIKER_position_band_right_hp</t>
-  </si>
-  <si>
-    <t>OETIKER_position_band_left_wp</t>
-  </si>
-  <si>
-    <t>OETIKER_position_band_right_wp</t>
-  </si>
-  <si>
-    <t>ST1-sen_latch_left</t>
-  </si>
-  <si>
-    <t>ST1-sen_latch_right</t>
+    <t>ST1-vsen_module_HP_down</t>
+  </si>
+  <si>
+    <t>ST1-vsen_module_HP2_down</t>
+  </si>
+  <si>
+    <t>ST1-vsen_module_WP_up</t>
+  </si>
+  <si>
+    <t>ST1-vsen_module_WP2_up</t>
+  </si>
+  <si>
+    <t>ST1-ez_module_HP_down</t>
+  </si>
+  <si>
+    <t>ST1-ez_module_WP_up</t>
+  </si>
+  <si>
+    <t>ST1-vsen_handle_HP_left</t>
+  </si>
+  <si>
+    <t>ST1-vsen_handle_WP_right</t>
+  </si>
+  <si>
+    <t>ST1-ez_handle_HP_left</t>
+  </si>
+  <si>
+    <t>ST1-ez_handle_WP_right</t>
+  </si>
+  <si>
+    <t>ST1-vsen_plug_HP_left</t>
+  </si>
+  <si>
+    <t>ST1-vsen_plug_WP_right</t>
+  </si>
+  <si>
+    <t>ST1-ez_plug_HP_left</t>
+  </si>
+  <si>
+    <t>ST1-ez_plug_WP_right</t>
+  </si>
+  <si>
+    <t>ST2-ez_airblow_WP_open</t>
+  </si>
+  <si>
+    <t>ST2-vsen_measurement_gt2_HP_up</t>
+  </si>
+  <si>
+    <t>ST2-vsen_measurement_gt2_WP_down</t>
+  </si>
+  <si>
+    <t>ST2-ez_measurement_gt2_HP_up</t>
+  </si>
+  <si>
+    <t>ST2-ez_measurement_gt2_WP_down</t>
+  </si>
+  <si>
+    <t>ST2-ez_measurement_gt2_BRAKE_RELEASE</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_plug_HP_right</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_plug_WP_left</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_plug_HP_right</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_plug_WP_left</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_generator_left_HP_down</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_generator_left_WP_up</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_generator_left_HP_down</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_generator_left_WP_up</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_generator_right_HP_down</t>
+  </si>
+  <si>
+    <t>ST2-vsen_pin_generator_right_WP_up</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_generator_right_HP_down</t>
+  </si>
+  <si>
+    <t>ST2-ez_pin_generator_right_WP_up</t>
+  </si>
+  <si>
+    <t>ST1-sen_screw_01</t>
+  </si>
+  <si>
+    <t>ST1-sen_screw_02</t>
+  </si>
+  <si>
+    <t>ST1-sen_screw_03</t>
+  </si>
+  <si>
+    <t>ST1-sen_screw_04</t>
+  </si>
+  <si>
+    <t>STA-sen_package</t>
+  </si>
+  <si>
+    <t>STB-sen_package</t>
+  </si>
+  <si>
+    <t>STA-sen_plug</t>
+  </si>
+  <si>
+    <t>STB-sen_plug</t>
+  </si>
+  <si>
+    <t>ST1-sen_nest_00</t>
+  </si>
+  <si>
+    <t>ST1-sen_nest_01</t>
+  </si>
+  <si>
+    <t>ST1-sen_nest_02</t>
+  </si>
+  <si>
+    <t>A-sen_table_00</t>
+  </si>
+  <si>
+    <t>A-sen_table_01</t>
+  </si>
+  <si>
+    <t>ST1-sen_scanner_left</t>
+  </si>
+  <si>
+    <t>ST1-sen_scanner_right</t>
+  </si>
+  <si>
+    <t>WEISS_on_position</t>
+  </si>
+  <si>
+    <t>WEISS_alarm</t>
+  </si>
+  <si>
+    <t>WEISS_start_permitted</t>
   </si>
   <si>
     <t>SAFETY_pressure_ok</t>
   </si>
   <si>
-    <t>SAFETY_blockade</t>
+    <t>SAFETY_phase_ok</t>
+  </si>
+  <si>
+    <t>SAFETY_table_ok</t>
+  </si>
+  <si>
+    <t>SAFETY_curtain_ok</t>
   </si>
   <si>
     <t>SAFETY_estop_ok</t>
   </si>
   <si>
+    <t>SAFETY_doors_closed</t>
+  </si>
+  <si>
     <t>A-btn_start</t>
   </si>
   <si>
@@ -151,9 +226,6 @@
     <t>A-btn_panel_red</t>
   </si>
   <si>
-    <t>A-btn_start_on_grip</t>
-  </si>
-  <si>
     <t>A-led_panel_white</t>
   </si>
   <si>
@@ -178,25 +250,76 @@
     <t>A-rel_light</t>
   </si>
   <si>
-    <t>Oetiker_clamping_ok</t>
-  </si>
-  <si>
-    <t>Oetiker_clamping_nok</t>
-  </si>
-  <si>
-    <t>Oetiker_start</t>
-  </si>
-  <si>
-    <t>Oetiker_program_00</t>
-  </si>
-  <si>
-    <t>Oetiker_program_01</t>
-  </si>
-  <si>
-    <t>Oetiker_program_02</t>
-  </si>
-  <si>
-    <t>Oetiker_program_03</t>
+    <t>A-rel_light_camera</t>
+  </si>
+  <si>
+    <t>SAFETY_curtain_autostart</t>
+  </si>
+  <si>
+    <t>WEISS_start_rotation</t>
+  </si>
+  <si>
+    <t>WEISS_stop_rotation</t>
+  </si>
+  <si>
+    <t>WEISS_release_brake</t>
+  </si>
+  <si>
+    <t>ISO-rel_measurement_permitted</t>
+  </si>
+  <si>
+    <t>ISO-rel_measurement_start</t>
+  </si>
+  <si>
+    <t>A-rel_primer_or_insulation</t>
+  </si>
+  <si>
+    <t>PRIMER-rel_measurement_permitted</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_start</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_reset</t>
+  </si>
+  <si>
+    <t>PRIMER_transfer</t>
+  </si>
+  <si>
+    <t>PRIMER_bin_00</t>
+  </si>
+  <si>
+    <t>PRIMER_bin_01</t>
+  </si>
+  <si>
+    <t>PRIMER_bin_02</t>
+  </si>
+  <si>
+    <t>PRIMER_bin_03</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_in_progress</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_finished</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_error</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_less_eq</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_less</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_eq</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_more</t>
+  </si>
+  <si>
+    <t>PRIMER_measurement_more_eq</t>
   </si>
   <si>
     <t>I0</t>
@@ -205,6 +328,9 @@
     <t>I1</t>
   </si>
   <si>
+    <t>I2</t>
+  </si>
+  <si>
     <t>I10</t>
   </si>
   <si>
@@ -217,16 +343,19 @@
     <t>I21</t>
   </si>
   <si>
+    <t>I30</t>
+  </si>
+  <si>
+    <t>I31</t>
+  </si>
+  <si>
     <t>Q0</t>
   </si>
   <si>
     <t>Q1</t>
   </si>
   <si>
-    <t>Q10</t>
-  </si>
-  <si>
-    <t>Q11</t>
+    <t>Q2</t>
   </si>
   <si>
     <t>Q20</t>
@@ -235,6 +364,12 @@
     <t>Q21</t>
   </si>
   <si>
+    <t>Q40</t>
+  </si>
+  <si>
+    <t>Q41</t>
+  </si>
+  <si>
     <t>io</t>
   </si>
   <si>
@@ -247,141 +382,213 @@
     <t>Byte</t>
   </si>
   <si>
+    <t>%I10.2</t>
+  </si>
+  <si>
+    <t>%I10.3</t>
+  </si>
+  <si>
+    <t>%I11.2</t>
+  </si>
+  <si>
+    <t>%I11.3</t>
+  </si>
+  <si>
+    <t>%Q20.5</t>
+  </si>
+  <si>
+    <t>%Q21.5</t>
+  </si>
+  <si>
+    <t>%I20.1</t>
+  </si>
+  <si>
+    <t>%I21.1</t>
+  </si>
+  <si>
+    <t>%Q20.6</t>
+  </si>
+  <si>
+    <t>%Q21.6</t>
+  </si>
+  <si>
+    <t>%I20.2</t>
+  </si>
+  <si>
+    <t>%I21.2</t>
+  </si>
+  <si>
+    <t>%Q20.7</t>
+  </si>
+  <si>
+    <t>%Q21.7</t>
+  </si>
+  <si>
+    <t>%Q40.3</t>
+  </si>
+  <si>
+    <t>%I30.1</t>
+  </si>
+  <si>
+    <t>%I31.1</t>
+  </si>
+  <si>
+    <t>%Q40.4</t>
+  </si>
+  <si>
+    <t>%Q41.4</t>
+  </si>
+  <si>
+    <t>%Q41.3</t>
+  </si>
+  <si>
+    <t>%I30.2</t>
+  </si>
+  <si>
+    <t>%I31.2</t>
+  </si>
+  <si>
+    <t>%Q40.5</t>
+  </si>
+  <si>
+    <t>%Q41.5</t>
+  </si>
+  <si>
+    <t>%I30.3</t>
+  </si>
+  <si>
+    <t>%I31.3</t>
+  </si>
+  <si>
+    <t>%Q40.6</t>
+  </si>
+  <si>
+    <t>%Q41.6</t>
+  </si>
+  <si>
+    <t>%I30.4</t>
+  </si>
+  <si>
+    <t>%I31.4</t>
+  </si>
+  <si>
+    <t>%Q40.7</t>
+  </si>
+  <si>
+    <t>%Q41.7</t>
+  </si>
+  <si>
+    <t>%I10.0</t>
+  </si>
+  <si>
+    <t>%I11.0</t>
+  </si>
+  <si>
     <t>%I10.1</t>
   </si>
   <si>
     <t>%I11.1</t>
   </si>
   <si>
-    <t>%Q10.7</t>
+    <t>%I10.4</t>
+  </si>
+  <si>
+    <t>%I11.4</t>
+  </si>
+  <si>
+    <t>%I10.5</t>
+  </si>
+  <si>
+    <t>%I11.5</t>
+  </si>
+  <si>
+    <t>%I10.6</t>
+  </si>
+  <si>
+    <t>%I11.6</t>
+  </si>
+  <si>
+    <t>%I10.7</t>
+  </si>
+  <si>
+    <t>%I30.0</t>
+  </si>
+  <si>
+    <t>%I31.0</t>
+  </si>
+  <si>
+    <t>%I20.0</t>
+  </si>
+  <si>
+    <t>%I21.0</t>
+  </si>
+  <si>
+    <t>%I1.1</t>
+  </si>
+  <si>
+    <t>%I1.2</t>
+  </si>
+  <si>
+    <t>%I1.3</t>
+  </si>
+  <si>
+    <t>%I0.1</t>
+  </si>
+  <si>
+    <t>%I0.2</t>
+  </si>
+  <si>
+    <t>%I0.3</t>
+  </si>
+  <si>
+    <t>%I0.4</t>
+  </si>
+  <si>
+    <t>%I0.5</t>
+  </si>
+  <si>
+    <t>%I1.0</t>
+  </si>
+  <si>
+    <t>%I0.0</t>
+  </si>
+  <si>
+    <t>%I0.6</t>
+  </si>
+  <si>
+    <t>%I0.7</t>
+  </si>
+  <si>
+    <t>%Q0.0</t>
+  </si>
+  <si>
+    <t>%Q0.1</t>
+  </si>
+  <si>
+    <t>%Q0.2</t>
+  </si>
+  <si>
+    <t>%Q0.3</t>
+  </si>
+  <si>
+    <t>%Q0.4</t>
+  </si>
+  <si>
+    <t>%Q0.5</t>
+  </si>
+  <si>
+    <t>%Q0.6</t>
   </si>
   <si>
     <t>%Q1.7</t>
   </si>
   <si>
-    <t>%Q11.7</t>
-  </si>
-  <si>
-    <t>%I20.4</t>
-  </si>
-  <si>
-    <t>%I21.4</t>
-  </si>
-  <si>
-    <t>%Q20.6</t>
-  </si>
-  <si>
-    <t>%Q21.6</t>
-  </si>
-  <si>
-    <t>%I20.5</t>
-  </si>
-  <si>
-    <t>%I21.5</t>
-  </si>
-  <si>
-    <t>%Q20.7</t>
-  </si>
-  <si>
-    <t>%Q21.7</t>
-  </si>
-  <si>
-    <t>%I1.3</t>
-  </si>
-  <si>
-    <t>%I1.4</t>
-  </si>
-  <si>
-    <t>%I10.0</t>
-  </si>
-  <si>
-    <t>%I11.0</t>
-  </si>
-  <si>
-    <t>%I10.3</t>
-  </si>
-  <si>
-    <t>%I20.0</t>
-  </si>
-  <si>
-    <t>%I10.2</t>
-  </si>
-  <si>
-    <t>%I11.2</t>
-  </si>
-  <si>
-    <t>%I11.3</t>
-  </si>
-  <si>
-    <t>%I20.1</t>
-  </si>
-  <si>
-    <t>%I21.1</t>
-  </si>
-  <si>
-    <t>%I20.2</t>
-  </si>
-  <si>
-    <t>%I21.2</t>
-  </si>
-  <si>
-    <t>%I20.3</t>
-  </si>
-  <si>
-    <t>%I21.3</t>
-  </si>
-  <si>
-    <t>%I0.1</t>
-  </si>
-  <si>
-    <t>%I0.4</t>
-  </si>
-  <si>
-    <t>%I0.5</t>
-  </si>
-  <si>
-    <t>%I0.0</t>
-  </si>
-  <si>
-    <t>%I0.6</t>
-  </si>
-  <si>
-    <t>%I0.7</t>
-  </si>
-  <si>
-    <t>%I1.2</t>
-  </si>
-  <si>
-    <t>%Q0.0</t>
-  </si>
-  <si>
-    <t>%Q0.1</t>
-  </si>
-  <si>
-    <t>%Q0.2</t>
-  </si>
-  <si>
-    <t>%Q0.3</t>
-  </si>
-  <si>
-    <t>%Q0.4</t>
-  </si>
-  <si>
-    <t>%Q0.5</t>
-  </si>
-  <si>
-    <t>%Q0.6</t>
+    <t>%Q2.7</t>
   </si>
   <si>
     <t>%Q0.7</t>
   </si>
   <si>
-    <t>%I1.0</t>
-  </si>
-  <si>
-    <t>%I1.1</t>
-  </si>
-  <si>
     <t>%Q1.0</t>
   </si>
   <si>
@@ -391,18 +598,72 @@
     <t>%Q1.2</t>
   </si>
   <si>
+    <t>%Q1.5</t>
+  </si>
+  <si>
+    <t>%Q1.6</t>
+  </si>
+  <si>
     <t>%Q1.3</t>
   </si>
   <si>
     <t>%Q1.4</t>
   </si>
   <si>
+    <t>%Q2.0</t>
+  </si>
+  <si>
+    <t>%Q2.1</t>
+  </si>
+  <si>
+    <t>%Q2.2</t>
+  </si>
+  <si>
+    <t>%Q2.3</t>
+  </si>
+  <si>
+    <t>%Q2.4</t>
+  </si>
+  <si>
+    <t>%Q2.5</t>
+  </si>
+  <si>
+    <t>%Q2.6</t>
+  </si>
+  <si>
+    <t>%I2.0</t>
+  </si>
+  <si>
+    <t>%I2.1</t>
+  </si>
+  <si>
+    <t>%I2.2</t>
+  </si>
+  <si>
+    <t>%I2.3</t>
+  </si>
+  <si>
+    <t>%I2.4</t>
+  </si>
+  <si>
+    <t>%I2.5</t>
+  </si>
+  <si>
+    <t>%I2.6</t>
+  </si>
+  <si>
+    <t>%I2.7</t>
+  </si>
+  <si>
     <t>IB0</t>
   </si>
   <si>
     <t>IB1</t>
   </si>
   <si>
+    <t>IB2</t>
+  </si>
+  <si>
     <t>IB10</t>
   </si>
   <si>
@@ -415,16 +676,19 @@
     <t>IB21</t>
   </si>
   <si>
+    <t>IB30</t>
+  </si>
+  <si>
+    <t>IB31</t>
+  </si>
+  <si>
     <t>QB0</t>
   </si>
   <si>
     <t>QB1</t>
   </si>
   <si>
-    <t>QB10</t>
-  </si>
-  <si>
-    <t>QB11</t>
+    <t>QB2</t>
   </si>
   <si>
     <t>QB20</t>
@@ -433,99 +697,180 @@
     <t>QB21</t>
   </si>
   <si>
-    <t>[I10.1] czujnik "GN-docisk" HP open</t>
-  </si>
-  <si>
-    <t>[I11.1] czujnik "GN-docisk" WP close</t>
-  </si>
-  <si>
-    <t>[1] GN-docisk HP open [I10.1]</t>
-  </si>
-  <si>
-    <t>[1] GN-docisk WP close [I11.1]</t>
-  </si>
-  <si>
-    <t>[1] GN-docisk IDLE</t>
-  </si>
-  <si>
-    <t>[I20.4] czujnik "ST1-blokada_lewa" HP down</t>
-  </si>
-  <si>
-    <t>[I21.4] czujnik "ST1-blokada_lewa" WP up</t>
-  </si>
-  <si>
-    <t>[2] ST1-blokada_lewa HP down [I20.4]</t>
-  </si>
-  <si>
-    <t>[2] ST1-blokada_lewa WP up [I21.4]</t>
-  </si>
-  <si>
-    <t>[I20.5] czujnik "ST1-blokada_prawa" HP down</t>
-  </si>
-  <si>
-    <t>[I21.5] czujnik "ST1-blokada_prawa" WP up</t>
-  </si>
-  <si>
-    <t>[3] ST1-blokada_prawa HP down [I20.5]</t>
-  </si>
-  <si>
-    <t>[3] ST1-blokada_prawa WP up [I21.5]</t>
-  </si>
-  <si>
-    <t>[I1.3] czujnik "A-sen_skaner_lewo"</t>
-  </si>
-  <si>
-    <t>[I1.4] czujnik "A-sen_skaner_prawo"</t>
-  </si>
-  <si>
-    <t>[I10.0] czujnik "GN-sen_stelaz_sruba_lewa"</t>
-  </si>
-  <si>
-    <t>[I11.0] czujnik "GN-sen_stelaz_sruba_prawa"</t>
-  </si>
-  <si>
-    <t>[I10.3] czujnik "GN-sen_generator_sruba"</t>
-  </si>
-  <si>
-    <t>[I20.0] czujnik "OETIKER_pozycja_hp"</t>
-  </si>
-  <si>
-    <t>[I10.2] czujnik "OETIKER_pozycja_2mm"</t>
-  </si>
-  <si>
-    <t>[I11.2] czujnik "OETIKER_pozycja_4mm"</t>
-  </si>
-  <si>
-    <t>[I11.3] czujnik "OETIKER_pozycja_tensometr"</t>
-  </si>
-  <si>
-    <t>[I20.1] czujnik "OETIKER_pozycja_opaska_lewa_hp"</t>
-  </si>
-  <si>
-    <t>[I21.1] czujnik "OETIKER_pozycja_opaska_prawa_hp"</t>
-  </si>
-  <si>
-    <t>[I20.2] czujnik "OETIKER_pozycja_opaska_lewa_wp"</t>
-  </si>
-  <si>
-    <t>[I21.2] czujnik "OETIKER_pozycja_opaska_prawa_wp"</t>
-  </si>
-  <si>
-    <t>[I20.3] czujnik "ST1-sen_zasuwka_lewo"</t>
-  </si>
-  <si>
-    <t>[I21.3] czujnik "ST1-sen_zasuwka_prawo"</t>
+    <t>QB40</t>
+  </si>
+  <si>
+    <t>QB41</t>
+  </si>
+  <si>
+    <t>[I10.2] czujnik "ST1-modul" HP down</t>
+  </si>
+  <si>
+    <t>[I10.3] czujnik "ST1-modul" HP down</t>
+  </si>
+  <si>
+    <t>[I11.2] czujnik "ST1-modul" WP up</t>
+  </si>
+  <si>
+    <t>[I11.3] czujnik "ST1-modul" WP up</t>
+  </si>
+  <si>
+    <t>[1] ST1-modul HP down [I10.2, I10.3]</t>
+  </si>
+  <si>
+    <t>[1] ST1-modul WP up [I11.2, I11.3]</t>
+  </si>
+  <si>
+    <t>[I20.1] czujnik "ST1-dzwignia" HP left</t>
+  </si>
+  <si>
+    <t>[I21.1] czujnik "ST1-dzwignia" WP right</t>
+  </si>
+  <si>
+    <t>[2] ST1-dzwignia HP left [I20.1]</t>
+  </si>
+  <si>
+    <t>[2] ST1-dzwignia WP right [I21.1]</t>
+  </si>
+  <si>
+    <t>[I20.2] czujnik "ST1-wtyczka" HP left</t>
+  </si>
+  <si>
+    <t>[I21.2] czujnik "ST1-wtyczka" WP right</t>
+  </si>
+  <si>
+    <t>[3] ST1-wtyczka HP left [I20.2]</t>
+  </si>
+  <si>
+    <t>[3] ST1-wtyczka WP right [I21.2]</t>
+  </si>
+  <si>
+    <t>[4] ST2-przedmuch WP open [an]</t>
+  </si>
+  <si>
+    <t>[I30.1] czujnik "ST2-pomiar_gt2" HP up</t>
+  </si>
+  <si>
+    <t>[I31.1] czujnik "ST2-pomiar_gt2" WP down</t>
+  </si>
+  <si>
+    <t>[5] ST2-pomiar_gt2 HP up [I30.1]</t>
+  </si>
+  <si>
+    <t>[5] ST2-pomiar_gt2 WP down [I31.1]</t>
+  </si>
+  <si>
+    <t>[5] ST2-pomiar_gt2 BRAKE RELEASE</t>
+  </si>
+  <si>
+    <t>[I30.2] czujnik "ST2-pin_wtyczka" HP right</t>
+  </si>
+  <si>
+    <t>[I31.2] czujnik "ST2-pin_wtyczka" WP left</t>
+  </si>
+  <si>
+    <t>[6] ST2-pin_wtyczka HP right [I30.2]</t>
+  </si>
+  <si>
+    <t>[6] ST2-pin_wtyczka WP left [I31.2]</t>
+  </si>
+  <si>
+    <t>[I30.3] czujnik "ST2-pin_generator_lewy" HP down</t>
+  </si>
+  <si>
+    <t>[I31.3] czujnik "ST2-pin_generator_lewy" WP up</t>
+  </si>
+  <si>
+    <t>[7] ST2-pin_generator_lewy HP down [I30.3]</t>
+  </si>
+  <si>
+    <t>[7] ST2-pin_generator_lewy WP up [I31.3]</t>
+  </si>
+  <si>
+    <t>[I30.4] czujnik "ST2-pin_generator_prawy" HP down</t>
+  </si>
+  <si>
+    <t>[I31.4] czujnik "ST2-pin_generator_prawy" WP up</t>
+  </si>
+  <si>
+    <t>[8] ST2-pin_generator_prawy HP down [I30.4]</t>
+  </si>
+  <si>
+    <t>[8] ST2-pin_generator_prawy WP up [I31.4]</t>
+  </si>
+  <si>
+    <t>[I10.0] czujnik "ST1-sen_sruba_01"</t>
+  </si>
+  <si>
+    <t>[I11.0] czujnik "ST1-sen_sruba_02"</t>
+  </si>
+  <si>
+    <t>[I10.1] czujnik "ST1-sen_sruba_03"</t>
+  </si>
+  <si>
+    <t>[I11.1] czujnik "ST1-sen_sruba_04"</t>
+  </si>
+  <si>
+    <t>[I10.4] czujnik "STA-sen_pakiet"</t>
+  </si>
+  <si>
+    <t>[I11.4] czujnik "STB-sen_pakiet"</t>
+  </si>
+  <si>
+    <t>[I10.5] czujnik "STA-sen_wtyczka"</t>
+  </si>
+  <si>
+    <t>[I11.5] czujnik "STB-sen_wtyczka"</t>
+  </si>
+  <si>
+    <t>[I10.6] czujnik "ST1-sen_gniazdo_00"</t>
+  </si>
+  <si>
+    <t>[I11.6] czujnik "ST1-sen_gniazdo_01"</t>
+  </si>
+  <si>
+    <t>[I10.7] czujnik "ST1-sen_gniazdo_02"</t>
+  </si>
+  <si>
+    <t>[I30.0] czujnik "A-sen_stol_00"</t>
+  </si>
+  <si>
+    <t>[I31.0] czujnik "A-sen_stol_01"</t>
+  </si>
+  <si>
+    <t>[I20.0] czujnik "ST1-sen_skaner_lewo"</t>
+  </si>
+  <si>
+    <t>[I21.0] czujnik "ST1-sen_skaner_prawo"</t>
+  </si>
+  <si>
+    <t>[I1.1] czujnik "WEISS_na_pozycji"</t>
+  </si>
+  <si>
+    <t>[I1.2] czujnik "WEISS_alarm"</t>
+  </si>
+  <si>
+    <t>[I1.3] czujnik "WEISS_zezwolenie_na_start"</t>
   </si>
   <si>
     <t>[I0.1]  "SAFETY_cisnienie_ok"</t>
   </si>
   <si>
-    <t>[I0.4]  "SAFETY_blokada"</t>
+    <t>[I0.2]  "SAFETY_faza_ok"</t>
+  </si>
+  <si>
+    <t>[I0.3]  "SAFETY_stol_ok"</t>
+  </si>
+  <si>
+    <t>[I0.4]  "SAFETY_kurtyna_ok"</t>
   </si>
   <si>
     <t>[I0.5]  "SAFETY_estop_ok"</t>
   </si>
   <si>
+    <t>[I1.0]  "SAFETY_drzwi_zamkniete"</t>
+  </si>
+  <si>
     <t>[I0.0] przycisk "A-btn_start"</t>
   </si>
   <si>
@@ -535,9 +880,6 @@
     <t>[I0.7] przycisk "A-btn_panel_czerwony"</t>
   </si>
   <si>
-    <t>[I1.2] przycisk "A-btn_start_na_uchwycie"</t>
-  </si>
-  <si>
     <t>[Q0.0]  "A-led_panel_bialy"</t>
   </si>
   <si>
@@ -559,28 +901,79 @@
     <t>[Q0.6]  "A-led_kolumna_zolty"</t>
   </si>
   <si>
-    <t>[Q0.7]  "A-rel_oswietlenie"</t>
-  </si>
-  <si>
-    <t>[I1.0]  "Oetiker_zaciskanie_ok"</t>
-  </si>
-  <si>
-    <t>[I1.1]  "Oetiker_zaciskanie_nok"</t>
-  </si>
-  <si>
-    <t>[Q1.0]  "Oetiker_start"</t>
-  </si>
-  <si>
-    <t>[Q1.1]  "Oetiker_program_00"</t>
-  </si>
-  <si>
-    <t>[Q1.2]  "Oetiker_program_01"</t>
-  </si>
-  <si>
-    <t>[Q1.3]  "Oetiker_program_02"</t>
-  </si>
-  <si>
-    <t>[Q1.4]  "Oetiker_program_03"</t>
+    <t>[Q1.7]  "A-rel_oswietlenie"</t>
+  </si>
+  <si>
+    <t>[Q2.7]  "A-rel_doswietlacz_kamery"</t>
+  </si>
+  <si>
+    <t>[Q0.7]  "SAFETY_kurtyna_autostart"</t>
+  </si>
+  <si>
+    <t>[Q1.0]  "WEISS_obrot_start"</t>
+  </si>
+  <si>
+    <t>[Q1.1]  "WEISS_obrot_stop"</t>
+  </si>
+  <si>
+    <t>[Q1.2]  "WEISS_zwolnik_hamulec"</t>
+  </si>
+  <si>
+    <t>[Q1.5]  "ISO-rel_pomiar_zezwolenie"</t>
+  </si>
+  <si>
+    <t>[Q1.6]  "ISO-rel_pomiar_start"</t>
+  </si>
+  <si>
+    <t>[Q1.3]  "A-rel_splonka_lub_izolacja"</t>
+  </si>
+  <si>
+    <t>[Q1.4]  "PRIMER-rel_pomiar_zezwolenie"</t>
+  </si>
+  <si>
+    <t>[Q2.0]  "PRIMER_pomiar_start"</t>
+  </si>
+  <si>
+    <t>[Q2.1]  "PRIMER_pomiar_reset"</t>
+  </si>
+  <si>
+    <t>[Q2.2]  "PRIMER_transfer"</t>
+  </si>
+  <si>
+    <t>[Q2.3]  "PRIMER_bin_00"</t>
+  </si>
+  <si>
+    <t>[Q2.4]  "PRIMER_bin_01"</t>
+  </si>
+  <si>
+    <t>[Q2.5]  "PRIMER_bin_02"</t>
+  </si>
+  <si>
+    <t>[Q2.6]  "PRIMER_bin_03"</t>
+  </si>
+  <si>
+    <t>[I2.0]  "PRIMER_pomiar_trwa"</t>
+  </si>
+  <si>
+    <t>[I2.1]  "PRIMER_pomiar_zakonczono"</t>
+  </si>
+  <si>
+    <t>[I2.2]  "PRIMER_pomiar_error"</t>
+  </si>
+  <si>
+    <t>[I2.3]  "PRIMER_pomiar_mniejszy_rowny"</t>
+  </si>
+  <si>
+    <t>[I2.4]  "PRIMER_pomiar_mniejszy"</t>
+  </si>
+  <si>
+    <t>[I2.5]  "PRIMER_pomiar_rowny"</t>
+  </si>
+  <si>
+    <t>[I2.6]  "PRIMER_pomiar_wiekszy"</t>
+  </si>
+  <si>
+    <t>[I2.7]  "PRIMER_pomiar_wiekszy_rowny"</t>
   </si>
   <si>
     <t>True</t>
@@ -941,7 +1334,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -987,25 +1380,25 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>229</v>
       </c>
       <c r="F2" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G2" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H2" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1013,25 +1406,25 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H3" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1039,25 +1432,25 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
       <c r="F4" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G4" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H4" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1065,25 +1458,25 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G5" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H5" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1091,25 +1484,25 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G6" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H6" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1117,25 +1510,25 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G7" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H7" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1143,25 +1536,25 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>235</v>
       </c>
       <c r="F8" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G8" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H8" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1169,25 +1562,25 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G9" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H9" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1195,25 +1588,25 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>237</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G10" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H10" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1221,25 +1614,25 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H11" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1247,25 +1640,25 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>239</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G12" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1273,25 +1666,25 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G13" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H13" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1299,25 +1692,25 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G14" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H14" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1325,25 +1718,25 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>242</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G15" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H15" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1351,25 +1744,25 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G16" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H16" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1377,25 +1770,25 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G17" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H17" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1403,25 +1796,25 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G18" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H18" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1429,25 +1822,25 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>246</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G19" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1455,25 +1848,25 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="F20" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G20" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H20" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1481,25 +1874,25 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>248</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G21" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H21" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1507,25 +1900,25 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="E22" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="F22" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G22" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H22" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1533,25 +1926,25 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G23" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H23" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1559,25 +1952,25 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="F24" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G24" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H24" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1585,25 +1978,25 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G25" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H25" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1611,25 +2004,25 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>163</v>
+        <v>253</v>
       </c>
       <c r="F26" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G26" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H26" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1637,25 +2030,25 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="F27" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G27" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H27" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1663,25 +2056,25 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G28" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H28" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1689,25 +2082,25 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G29" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H29" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1715,25 +2108,25 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G30" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H30" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1741,25 +2134,25 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
+        <v>258</v>
       </c>
       <c r="F31" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G31" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H31" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1767,25 +2160,25 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="E32" t="s">
-        <v>169</v>
+        <v>259</v>
       </c>
       <c r="F32" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G32" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H32" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1793,25 +2186,25 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="F33" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G33" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H33" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1819,25 +2212,25 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
+        <v>261</v>
       </c>
       <c r="F34" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G34" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H34" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1845,25 +2238,25 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G35" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H35" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1871,25 +2264,25 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="F36" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G36" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H36" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1897,25 +2290,25 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="F37" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G37" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H37" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1923,25 +2316,25 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="E38" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="F38" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G38" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H38" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1949,25 +2342,25 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="F39" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G39" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H39" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1975,25 +2368,25 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="F40" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G40" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H40" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2001,25 +2394,25 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="E41" t="s">
-        <v>178</v>
+        <v>268</v>
       </c>
       <c r="F41" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G41" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H41" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2027,25 +2420,25 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="E42" t="s">
-        <v>179</v>
+        <v>269</v>
       </c>
       <c r="F42" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G42" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H42" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2053,25 +2446,25 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="F43" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G43" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H43" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2079,25 +2472,25 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D44" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="E44" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F44" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G44" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H44" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2105,25 +2498,25 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="E45" t="s">
-        <v>182</v>
+        <v>272</v>
       </c>
       <c r="F45" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G45" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H45" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2131,25 +2524,25 @@
         <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D46" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="E46" t="s">
-        <v>183</v>
+        <v>273</v>
       </c>
       <c r="F46" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G46" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H46" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2157,25 +2550,25 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>274</v>
       </c>
       <c r="F47" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G47" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H47" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2183,25 +2576,25 @@
         <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="E48" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="F48" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G48" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H48" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2209,25 +2602,25 @@
         <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="E49" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="F49" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G49" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H49" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2235,25 +2628,25 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="E50" t="s">
-        <v>187</v>
+        <v>277</v>
       </c>
       <c r="F50" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G50" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H50" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2261,25 +2654,25 @@
         <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>188</v>
+        <v>278</v>
       </c>
       <c r="F51" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G51" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H51" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2287,25 +2680,25 @@
         <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>279</v>
       </c>
       <c r="F52" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G52" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H52" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2313,25 +2706,25 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="E53" t="s">
-        <v>128</v>
+        <v>280</v>
       </c>
       <c r="F53" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G53" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H53" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2339,25 +2732,25 @@
         <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="E54" t="s">
-        <v>129</v>
+        <v>281</v>
       </c>
       <c r="F54" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G54" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H54" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2365,25 +2758,25 @@
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D55" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>282</v>
       </c>
       <c r="F55" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G55" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H55" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2391,25 +2784,25 @@
         <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="E56" t="s">
-        <v>131</v>
+        <v>283</v>
       </c>
       <c r="F56" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G56" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H56" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2417,25 +2810,25 @@
         <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="E57" t="s">
-        <v>132</v>
+        <v>284</v>
       </c>
       <c r="F57" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G57" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H57" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2443,25 +2836,25 @@
         <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="E58" t="s">
-        <v>133</v>
+        <v>285</v>
       </c>
       <c r="F58" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G58" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H58" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2469,25 +2862,25 @@
         <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D59" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="E59" t="s">
-        <v>134</v>
+        <v>286</v>
       </c>
       <c r="F59" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G59" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H59" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2495,25 +2888,25 @@
         <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D60" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="E60" t="s">
-        <v>135</v>
+        <v>287</v>
       </c>
       <c r="F60" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G60" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H60" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2521,25 +2914,25 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D61" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="E61" t="s">
-        <v>136</v>
+        <v>288</v>
       </c>
       <c r="F61" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G61" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H61" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2547,25 +2940,25 @@
         <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="E62" t="s">
-        <v>137</v>
+        <v>289</v>
       </c>
       <c r="F62" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="G62" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
       <c r="H62" t="s">
-        <v>189</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2573,25 +2966,1195 @@
         <v>72</v>
       </c>
       <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" t="s">
+        <v>290</v>
+      </c>
+      <c r="F63" t="s">
+        <v>320</v>
+      </c>
+      <c r="G63" t="s">
+        <v>320</v>
+      </c>
+      <c r="H63" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" t="s">
+        <v>291</v>
+      </c>
+      <c r="F64" t="s">
+        <v>320</v>
+      </c>
+      <c r="G64" t="s">
+        <v>320</v>
+      </c>
+      <c r="H64" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
         <v>74</v>
       </c>
-      <c r="C63" t="s">
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" t="s">
+        <v>292</v>
+      </c>
+      <c r="F65" t="s">
+        <v>320</v>
+      </c>
+      <c r="G65" t="s">
+        <v>320</v>
+      </c>
+      <c r="H65" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" t="s">
+        <v>120</v>
+      </c>
+      <c r="D66" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" t="s">
+        <v>293</v>
+      </c>
+      <c r="F66" t="s">
+        <v>320</v>
+      </c>
+      <c r="G66" t="s">
+        <v>320</v>
+      </c>
+      <c r="H66" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
         <v>76</v>
       </c>
-      <c r="D63" t="s">
-        <v>138</v>
-      </c>
-      <c r="E63" t="s">
-        <v>138</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" t="s">
+        <v>294</v>
+      </c>
+      <c r="F67" t="s">
+        <v>320</v>
+      </c>
+      <c r="G67" t="s">
+        <v>320</v>
+      </c>
+      <c r="H67" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" t="s">
+        <v>118</v>
+      </c>
+      <c r="C68" t="s">
+        <v>120</v>
+      </c>
+      <c r="D68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" t="s">
+        <v>295</v>
+      </c>
+      <c r="F68" t="s">
+        <v>320</v>
+      </c>
+      <c r="G68" t="s">
+        <v>320</v>
+      </c>
+      <c r="H68" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D69" t="s">
         <v>189</v>
       </c>
-      <c r="G63" t="s">
-        <v>189</v>
-      </c>
-      <c r="H63" t="s">
-        <v>189</v>
+      <c r="E69" t="s">
+        <v>296</v>
+      </c>
+      <c r="F69" t="s">
+        <v>320</v>
+      </c>
+      <c r="G69" t="s">
+        <v>320</v>
+      </c>
+      <c r="H69" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" t="s">
+        <v>190</v>
+      </c>
+      <c r="E70" t="s">
+        <v>297</v>
+      </c>
+      <c r="F70" t="s">
+        <v>320</v>
+      </c>
+      <c r="G70" t="s">
+        <v>320</v>
+      </c>
+      <c r="H70" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" t="s">
+        <v>120</v>
+      </c>
+      <c r="D71" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" t="s">
+        <v>298</v>
+      </c>
+      <c r="F71" t="s">
+        <v>320</v>
+      </c>
+      <c r="G71" t="s">
+        <v>320</v>
+      </c>
+      <c r="H71" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" t="s">
+        <v>192</v>
+      </c>
+      <c r="E72" t="s">
+        <v>299</v>
+      </c>
+      <c r="F72" t="s">
+        <v>320</v>
+      </c>
+      <c r="G72" t="s">
+        <v>320</v>
+      </c>
+      <c r="H72" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" t="s">
+        <v>120</v>
+      </c>
+      <c r="D73" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" t="s">
+        <v>300</v>
+      </c>
+      <c r="F73" t="s">
+        <v>320</v>
+      </c>
+      <c r="G73" t="s">
+        <v>320</v>
+      </c>
+      <c r="H73" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" t="s">
+        <v>301</v>
+      </c>
+      <c r="F74" t="s">
+        <v>320</v>
+      </c>
+      <c r="G74" t="s">
+        <v>320</v>
+      </c>
+      <c r="H74" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" t="s">
+        <v>302</v>
+      </c>
+      <c r="F75" t="s">
+        <v>320</v>
+      </c>
+      <c r="G75" t="s">
+        <v>320</v>
+      </c>
+      <c r="H75" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" t="s">
+        <v>120</v>
+      </c>
+      <c r="D76" t="s">
+        <v>196</v>
+      </c>
+      <c r="E76" t="s">
+        <v>303</v>
+      </c>
+      <c r="F76" t="s">
+        <v>320</v>
+      </c>
+      <c r="G76" t="s">
+        <v>320</v>
+      </c>
+      <c r="H76" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" t="s">
+        <v>120</v>
+      </c>
+      <c r="D77" t="s">
+        <v>197</v>
+      </c>
+      <c r="E77" t="s">
+        <v>304</v>
+      </c>
+      <c r="F77" t="s">
+        <v>320</v>
+      </c>
+      <c r="G77" t="s">
+        <v>320</v>
+      </c>
+      <c r="H77" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" t="s">
+        <v>198</v>
+      </c>
+      <c r="E78" t="s">
+        <v>305</v>
+      </c>
+      <c r="F78" t="s">
+        <v>320</v>
+      </c>
+      <c r="G78" t="s">
+        <v>320</v>
+      </c>
+      <c r="H78" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>88</v>
+      </c>
+      <c r="B79" t="s">
+        <v>118</v>
+      </c>
+      <c r="C79" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" t="s">
+        <v>199</v>
+      </c>
+      <c r="E79" t="s">
+        <v>306</v>
+      </c>
+      <c r="F79" t="s">
+        <v>320</v>
+      </c>
+      <c r="G79" t="s">
+        <v>320</v>
+      </c>
+      <c r="H79" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" t="s">
+        <v>200</v>
+      </c>
+      <c r="E80" t="s">
+        <v>307</v>
+      </c>
+      <c r="F80" t="s">
+        <v>320</v>
+      </c>
+      <c r="G80" t="s">
+        <v>320</v>
+      </c>
+      <c r="H80" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" t="s">
+        <v>201</v>
+      </c>
+      <c r="E81" t="s">
+        <v>308</v>
+      </c>
+      <c r="F81" t="s">
+        <v>320</v>
+      </c>
+      <c r="G81" t="s">
+        <v>320</v>
+      </c>
+      <c r="H81" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" t="s">
+        <v>120</v>
+      </c>
+      <c r="D82" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82" t="s">
+        <v>309</v>
+      </c>
+      <c r="F82" t="s">
+        <v>320</v>
+      </c>
+      <c r="G82" t="s">
+        <v>320</v>
+      </c>
+      <c r="H82" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" t="s">
+        <v>120</v>
+      </c>
+      <c r="D83" t="s">
+        <v>203</v>
+      </c>
+      <c r="E83" t="s">
+        <v>310</v>
+      </c>
+      <c r="F83" t="s">
+        <v>320</v>
+      </c>
+      <c r="G83" t="s">
+        <v>320</v>
+      </c>
+      <c r="H83" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" t="s">
+        <v>120</v>
+      </c>
+      <c r="D84" t="s">
+        <v>204</v>
+      </c>
+      <c r="E84" t="s">
+        <v>311</v>
+      </c>
+      <c r="F84" t="s">
+        <v>320</v>
+      </c>
+      <c r="G84" t="s">
+        <v>320</v>
+      </c>
+      <c r="H84" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" t="s">
+        <v>205</v>
+      </c>
+      <c r="E85" t="s">
+        <v>312</v>
+      </c>
+      <c r="F85" t="s">
+        <v>320</v>
+      </c>
+      <c r="G85" t="s">
+        <v>320</v>
+      </c>
+      <c r="H85" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>120</v>
+      </c>
+      <c r="D86" t="s">
+        <v>206</v>
+      </c>
+      <c r="E86" t="s">
+        <v>313</v>
+      </c>
+      <c r="F86" t="s">
+        <v>320</v>
+      </c>
+      <c r="G86" t="s">
+        <v>320</v>
+      </c>
+      <c r="H86" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" t="s">
+        <v>120</v>
+      </c>
+      <c r="D87" t="s">
+        <v>207</v>
+      </c>
+      <c r="E87" t="s">
+        <v>314</v>
+      </c>
+      <c r="F87" t="s">
+        <v>320</v>
+      </c>
+      <c r="G87" t="s">
+        <v>320</v>
+      </c>
+      <c r="H87" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D88" t="s">
+        <v>208</v>
+      </c>
+      <c r="E88" t="s">
+        <v>315</v>
+      </c>
+      <c r="F88" t="s">
+        <v>320</v>
+      </c>
+      <c r="G88" t="s">
+        <v>320</v>
+      </c>
+      <c r="H88" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89" t="s">
+        <v>120</v>
+      </c>
+      <c r="D89" t="s">
+        <v>209</v>
+      </c>
+      <c r="E89" t="s">
+        <v>316</v>
+      </c>
+      <c r="F89" t="s">
+        <v>320</v>
+      </c>
+      <c r="G89" t="s">
+        <v>320</v>
+      </c>
+      <c r="H89" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" t="s">
+        <v>120</v>
+      </c>
+      <c r="D90" t="s">
+        <v>210</v>
+      </c>
+      <c r="E90" t="s">
+        <v>317</v>
+      </c>
+      <c r="F90" t="s">
+        <v>320</v>
+      </c>
+      <c r="G90" t="s">
+        <v>320</v>
+      </c>
+      <c r="H90" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" t="s">
+        <v>211</v>
+      </c>
+      <c r="E91" t="s">
+        <v>318</v>
+      </c>
+      <c r="F91" t="s">
+        <v>320</v>
+      </c>
+      <c r="G91" t="s">
+        <v>320</v>
+      </c>
+      <c r="H91" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" t="s">
+        <v>212</v>
+      </c>
+      <c r="E92" t="s">
+        <v>319</v>
+      </c>
+      <c r="F92" t="s">
+        <v>320</v>
+      </c>
+      <c r="G92" t="s">
+        <v>320</v>
+      </c>
+      <c r="H92" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" t="s">
+        <v>119</v>
+      </c>
+      <c r="C93" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" t="s">
+        <v>213</v>
+      </c>
+      <c r="E93" t="s">
+        <v>213</v>
+      </c>
+      <c r="F93" t="s">
+        <v>320</v>
+      </c>
+      <c r="G93" t="s">
+        <v>320</v>
+      </c>
+      <c r="H93" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94" t="s">
+        <v>121</v>
+      </c>
+      <c r="D94" t="s">
+        <v>214</v>
+      </c>
+      <c r="E94" t="s">
+        <v>214</v>
+      </c>
+      <c r="F94" t="s">
+        <v>320</v>
+      </c>
+      <c r="G94" t="s">
+        <v>320</v>
+      </c>
+      <c r="H94" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" t="s">
+        <v>215</v>
+      </c>
+      <c r="E95" t="s">
+        <v>215</v>
+      </c>
+      <c r="F95" t="s">
+        <v>320</v>
+      </c>
+      <c r="G95" t="s">
+        <v>320</v>
+      </c>
+      <c r="H95" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" t="s">
+        <v>119</v>
+      </c>
+      <c r="C96" t="s">
+        <v>121</v>
+      </c>
+      <c r="D96" t="s">
+        <v>216</v>
+      </c>
+      <c r="E96" t="s">
+        <v>216</v>
+      </c>
+      <c r="F96" t="s">
+        <v>320</v>
+      </c>
+      <c r="G96" t="s">
+        <v>320</v>
+      </c>
+      <c r="H96" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" t="s">
+        <v>217</v>
+      </c>
+      <c r="E97" t="s">
+        <v>217</v>
+      </c>
+      <c r="F97" t="s">
+        <v>320</v>
+      </c>
+      <c r="G97" t="s">
+        <v>320</v>
+      </c>
+      <c r="H97" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98" t="s">
+        <v>119</v>
+      </c>
+      <c r="C98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98" t="s">
+        <v>218</v>
+      </c>
+      <c r="E98" t="s">
+        <v>218</v>
+      </c>
+      <c r="F98" t="s">
+        <v>320</v>
+      </c>
+      <c r="G98" t="s">
+        <v>320</v>
+      </c>
+      <c r="H98" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" t="s">
+        <v>119</v>
+      </c>
+      <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" t="s">
+        <v>219</v>
+      </c>
+      <c r="E99" t="s">
+        <v>219</v>
+      </c>
+      <c r="F99" t="s">
+        <v>320</v>
+      </c>
+      <c r="G99" t="s">
+        <v>320</v>
+      </c>
+      <c r="H99" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100" t="s">
+        <v>220</v>
+      </c>
+      <c r="F100" t="s">
+        <v>320</v>
+      </c>
+      <c r="G100" t="s">
+        <v>320</v>
+      </c>
+      <c r="H100" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" t="s">
+        <v>119</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" t="s">
+        <v>221</v>
+      </c>
+      <c r="E101" t="s">
+        <v>221</v>
+      </c>
+      <c r="F101" t="s">
+        <v>320</v>
+      </c>
+      <c r="G101" t="s">
+        <v>320</v>
+      </c>
+      <c r="H101" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102" t="s">
+        <v>119</v>
+      </c>
+      <c r="C102" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102" t="s">
+        <v>222</v>
+      </c>
+      <c r="E102" t="s">
+        <v>222</v>
+      </c>
+      <c r="F102" t="s">
+        <v>320</v>
+      </c>
+      <c r="G102" t="s">
+        <v>320</v>
+      </c>
+      <c r="H102" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>112</v>
+      </c>
+      <c r="B103" t="s">
+        <v>119</v>
+      </c>
+      <c r="C103" t="s">
+        <v>121</v>
+      </c>
+      <c r="D103" t="s">
+        <v>223</v>
+      </c>
+      <c r="E103" t="s">
+        <v>223</v>
+      </c>
+      <c r="F103" t="s">
+        <v>320</v>
+      </c>
+      <c r="G103" t="s">
+        <v>320</v>
+      </c>
+      <c r="H103" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104" t="s">
+        <v>119</v>
+      </c>
+      <c r="C104" t="s">
+        <v>121</v>
+      </c>
+      <c r="D104" t="s">
+        <v>224</v>
+      </c>
+      <c r="E104" t="s">
+        <v>224</v>
+      </c>
+      <c r="F104" t="s">
+        <v>320</v>
+      </c>
+      <c r="G104" t="s">
+        <v>320</v>
+      </c>
+      <c r="H104" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105" t="s">
+        <v>225</v>
+      </c>
+      <c r="E105" t="s">
+        <v>225</v>
+      </c>
+      <c r="F105" t="s">
+        <v>320</v>
+      </c>
+      <c r="G105" t="s">
+        <v>320</v>
+      </c>
+      <c r="H105" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106" t="s">
+        <v>119</v>
+      </c>
+      <c r="C106" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106" t="s">
+        <v>226</v>
+      </c>
+      <c r="E106" t="s">
+        <v>226</v>
+      </c>
+      <c r="F106" t="s">
+        <v>320</v>
+      </c>
+      <c r="G106" t="s">
+        <v>320</v>
+      </c>
+      <c r="H106" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" t="s">
+        <v>119</v>
+      </c>
+      <c r="C107" t="s">
+        <v>121</v>
+      </c>
+      <c r="D107" t="s">
+        <v>227</v>
+      </c>
+      <c r="E107" t="s">
+        <v>227</v>
+      </c>
+      <c r="F107" t="s">
+        <v>320</v>
+      </c>
+      <c r="G107" t="s">
+        <v>320</v>
+      </c>
+      <c r="H107" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" t="s">
+        <v>121</v>
+      </c>
+      <c r="D108" t="s">
+        <v>228</v>
+      </c>
+      <c r="E108" t="s">
+        <v>228</v>
+      </c>
+      <c r="F108" t="s">
+        <v>320</v>
+      </c>
+      <c r="G108" t="s">
+        <v>320</v>
+      </c>
+      <c r="H108" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>